<commit_message>
Update Kicad project for rev.F
</commit_message>
<xml_diff>
--- a/kicad/opl3module/fabrication/opl3module-BOM.xlsx
+++ b/kicad/opl3module/fabrication/opl3module-BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>Comment</t>
   </si>
@@ -97,7 +97,7 @@
     <t>R1,R6,R11,R16,R21,R26</t>
   </si>
   <si>
-    <t>C138002</t>
+    <t>C25105</t>
   </si>
   <si>
     <t>6.8k</t>
@@ -118,6 +118,30 @@
     <t>C138071</t>
   </si>
   <si>
+    <t>YMF262</t>
+  </si>
+  <si>
+    <t>U1,U4,U7,U10,U13,U16</t>
+  </si>
+  <si>
+    <t>U_SOP-24_8.4x15.5mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>C9900016870</t>
+  </si>
+  <si>
+    <t>YAC512</t>
+  </si>
+  <si>
+    <t>U2,U5,U8,U11,U14,U17</t>
+  </si>
+  <si>
+    <t>U_SOP-16_5.3x10.2mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>C9900130385</t>
+  </si>
+  <si>
     <t>TL074</t>
   </si>
   <si>
@@ -136,10 +160,10 @@
     <t>XO1,XO2,XO3,XO4,XO5,XO6</t>
   </si>
   <si>
-    <t>XO_SMD5032</t>
-  </si>
-  <si>
-    <t>C387230</t>
+    <t>XO_SMD7050</t>
+  </si>
+  <si>
+    <t>C41988065</t>
   </si>
 </sst>
 </file>
@@ -149,7 +173,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -161,13 +185,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,12 +217,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -221,6 +256,19 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
@@ -266,6 +314,17 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
@@ -303,6 +362,19 @@
       </top>
       <bottom style="thin">
         <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -312,38 +384,47 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -366,6 +447,8 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ff56c1fe"/>
     </indexedColors>
@@ -384,10 +467,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -564,11 +647,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -577,33 +663,33 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -842,12 +928,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1128,7 +1214,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1399,17 +1485,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="13.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="48.5156" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.4062" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.9375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="2" max="2" width="48.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.35156" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1425,160 +1512,202 @@
       <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="4">
         <v>4</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="C2" t="s" s="6">
         <v>6</v>
       </c>
-      <c r="D2" t="s" s="6">
+      <c r="D2" t="s" s="7">
         <v>7</v>
       </c>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="7">
+      <c r="A3" t="s" s="9">
         <v>8</v>
       </c>
-      <c r="B3" t="s" s="8">
+      <c r="B3" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="C3" t="s" s="9">
+      <c r="C3" t="s" s="11">
         <v>6</v>
       </c>
-      <c r="D3" t="s" s="10">
+      <c r="D3" t="s" s="12">
         <v>10</v>
       </c>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="7">
+      <c r="A4" t="s" s="9">
         <v>11</v>
       </c>
-      <c r="B4" t="s" s="8">
+      <c r="B4" t="s" s="10">
         <v>12</v>
       </c>
-      <c r="C4" t="s" s="9">
+      <c r="C4" t="s" s="11">
         <v>13</v>
       </c>
-      <c r="D4" t="s" s="10">
+      <c r="D4" t="s" s="12">
         <v>14</v>
       </c>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="7">
+      <c r="A5" t="s" s="9">
         <v>15</v>
       </c>
-      <c r="B5" t="s" s="8">
+      <c r="B5" t="s" s="10">
         <v>16</v>
       </c>
-      <c r="C5" t="s" s="9">
+      <c r="C5" t="s" s="11">
         <v>13</v>
       </c>
-      <c r="D5" t="s" s="10">
+      <c r="D5" t="s" s="12">
         <v>17</v>
       </c>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="7">
+      <c r="A6" t="s" s="9">
         <v>18</v>
       </c>
-      <c r="B6" t="s" s="8">
+      <c r="B6" t="s" s="10">
         <v>19</v>
       </c>
-      <c r="C6" t="s" s="9">
+      <c r="C6" t="s" s="11">
         <v>20</v>
       </c>
-      <c r="D6" t="s" s="10">
+      <c r="D6" t="s" s="12">
         <v>21</v>
       </c>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="7">
+      <c r="A7" t="s" s="9">
         <v>22</v>
       </c>
-      <c r="B7" t="s" s="8">
+      <c r="B7" t="s" s="10">
         <v>23</v>
       </c>
-      <c r="C7" t="s" s="9">
+      <c r="C7" t="s" s="11">
         <v>24</v>
       </c>
-      <c r="D7" t="s" s="10">
+      <c r="D7" t="s" s="12">
         <v>25</v>
       </c>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="7">
+      <c r="A8" t="s" s="9">
         <v>26</v>
       </c>
-      <c r="B8" t="s" s="8">
+      <c r="B8" t="s" s="10">
         <v>27</v>
       </c>
-      <c r="C8" t="s" s="9">
+      <c r="C8" t="s" s="11">
         <v>20</v>
       </c>
-      <c r="D8" t="s" s="10">
+      <c r="D8" t="s" s="12">
         <v>28</v>
       </c>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="7">
+      <c r="A9" t="s" s="9">
         <v>29</v>
       </c>
-      <c r="B9" t="s" s="8">
+      <c r="B9" t="s" s="10">
         <v>30</v>
       </c>
-      <c r="C9" t="s" s="9">
+      <c r="C9" t="s" s="11">
         <v>20</v>
       </c>
-      <c r="D9" t="s" s="10">
+      <c r="D9" t="s" s="12">
         <v>31</v>
       </c>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="7">
+      <c r="A10" t="s" s="9">
         <v>32</v>
       </c>
-      <c r="B10" t="s" s="8">
+      <c r="B10" t="s" s="10">
         <v>33</v>
       </c>
-      <c r="C10" t="s" s="9">
+      <c r="C10" t="s" s="11">
         <v>20</v>
       </c>
-      <c r="D10" t="s" s="10">
+      <c r="D10" t="s" s="12">
         <v>34</v>
       </c>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="7">
+      <c r="A11" t="s" s="9">
         <v>35</v>
       </c>
-      <c r="B11" t="s" s="8">
+      <c r="B11" t="s" s="10">
         <v>36</v>
       </c>
-      <c r="C11" t="s" s="9">
+      <c r="C11" t="s" s="11">
         <v>37</v>
       </c>
-      <c r="D11" t="s" s="10">
+      <c r="D11" t="s" s="12">
         <v>38</v>
       </c>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="7">
+      <c r="A12" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="B12" t="s" s="8">
+      <c r="B12" t="s" s="10">
         <v>40</v>
       </c>
-      <c r="C12" t="s" s="9">
+      <c r="C12" t="s" s="11">
         <v>41</v>
       </c>
-      <c r="D12" t="s" s="10">
+      <c r="D12" t="s" s="12">
         <v>42</v>
       </c>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" t="s" s="9">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s" s="10">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s" s="11">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s" s="12">
+        <v>46</v>
+      </c>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" t="s" s="9">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s" s="10">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s" s="11">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s" s="12">
+        <v>50</v>
+      </c>
+      <c r="E14" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>